<commit_message>
actualizacion  Listado de reportes activos.xlsx
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes activos.xlsx
+++ b/00-Documentacion/Listado de reportes activos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4162DC2-F9A8-4A7D-8B75-61AFA9958092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8333BD-531F-4058-BA60-5BE42977ABD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="1120">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -3370,9 +3370,6 @@
   </si>
   <si>
     <t>zip,pdf,corre,excel</t>
-  </si>
-  <si>
-    <t>ws,ftp,pdf,correo,excel</t>
   </si>
   <si>
     <t>correo, excel,factura</t>
@@ -3395,6 +3392,12 @@
   </si>
   <si>
     <t>excel,correo,ftp,zip,xml, pdf</t>
+  </si>
+  <si>
+    <t>pdf,correo,excel,zip</t>
+  </si>
+  <si>
+    <t>ws,ftp,pdf,correo,excel,zip</t>
   </si>
 </sst>
 </file>
@@ -3834,8 +3837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361EBCA0-C102-45D9-BE91-837AD7D26F73}">
   <dimension ref="A1:H1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3864,7 +3867,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>38</v>
@@ -8004,7 +8007,7 @@
         <v>5</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="6" t="s">
@@ -8026,7 +8029,7 @@
         <v>5</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F190" s="6"/>
       <c r="G190" s="6" t="s">
@@ -8048,7 +8051,7 @@
         <v>5</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F191" s="6"/>
       <c r="G191" s="6" t="s">
@@ -8070,7 +8073,7 @@
         <v>5</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F192" s="6"/>
       <c r="G192" s="6" t="s">
@@ -8092,7 +8095,7 @@
         <v>5</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F193" s="6"/>
       <c r="G193" s="6" t="s">
@@ -8114,7 +8117,7 @@
         <v>5</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F194" s="6"/>
       <c r="G194" s="6" t="s">
@@ -8136,7 +8139,7 @@
         <v>5</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F195" s="6"/>
       <c r="G195" s="6" t="s">
@@ -8158,7 +8161,7 @@
         <v>5</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="6" t="s">
@@ -8180,7 +8183,7 @@
         <v>5</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="6" t="s">
@@ -8202,7 +8205,7 @@
         <v>5</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="6" t="s">
@@ -8224,7 +8227,7 @@
         <v>5</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="6" t="s">
@@ -8246,7 +8249,7 @@
         <v>5</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="6" t="s">
@@ -8268,7 +8271,7 @@
         <v>5</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="6" t="s">
@@ -8290,7 +8293,7 @@
         <v>5</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="6" t="s">
@@ -8312,7 +8315,7 @@
         <v>5</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F203" s="6"/>
       <c r="G203" s="6" t="s">
@@ -8334,7 +8337,7 @@
         <v>5</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F204" s="6"/>
       <c r="G204" s="6" t="s">
@@ -8356,7 +8359,7 @@
         <v>5</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F205" s="6"/>
       <c r="G205" s="6" t="s">
@@ -8620,7 +8623,7 @@
         <v>5</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F217" s="6"/>
       <c r="G217" s="6" t="s">
@@ -8642,7 +8645,7 @@
         <v>5</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F218" s="6"/>
       <c r="G218" s="6" t="s">
@@ -8664,7 +8667,7 @@
         <v>5</v>
       </c>
       <c r="E219" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="6" t="s">
@@ -8686,7 +8689,7 @@
         <v>5</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F220" s="6"/>
       <c r="G220" s="6" t="s">
@@ -8710,7 +8713,7 @@
         <v>5</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="6" t="s">
@@ -8734,7 +8737,7 @@
         <v>5</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F222" s="6"/>
       <c r="G222" s="6" t="s">
@@ -8758,7 +8761,7 @@
         <v>5</v>
       </c>
       <c r="E223" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F223" s="6"/>
       <c r="G223" s="6" t="s">
@@ -8782,7 +8785,7 @@
         <v>5</v>
       </c>
       <c r="E224" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F224" s="6"/>
       <c r="G224" s="6" t="s">
@@ -8806,7 +8809,7 @@
         <v>5</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F225" s="6"/>
       <c r="G225" s="6" t="s">
@@ -8830,7 +8833,7 @@
         <v>5</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F226" s="6"/>
       <c r="G226" s="6" t="s">
@@ -8854,7 +8857,7 @@
         <v>5</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F227" s="6"/>
       <c r="G227" s="6" t="s">
@@ -8878,7 +8881,7 @@
         <v>5</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F228" s="6"/>
       <c r="G228" s="6" t="s">
@@ -9480,7 +9483,7 @@
         <v>5</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F255" s="6"/>
       <c r="G255" s="6" t="s">
@@ -9524,7 +9527,7 @@
         <v>5</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F257" s="6"/>
       <c r="G257" s="6" t="s">
@@ -9546,7 +9549,7 @@
         <v>5</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F258" s="6"/>
       <c r="G258" s="6" t="s">
@@ -9568,7 +9571,7 @@
         <v>5</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F259" s="6"/>
       <c r="G259" s="6" t="s">
@@ -9590,7 +9593,7 @@
         <v>5</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F260" s="6"/>
       <c r="G260" s="6" t="s">
@@ -9612,7 +9615,7 @@
         <v>5</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F261" s="6"/>
       <c r="G261" s="6" t="s">
@@ -9634,7 +9637,7 @@
         <v>5</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F262" s="6"/>
       <c r="G262" s="6" t="s">
@@ -9656,7 +9659,7 @@
         <v>5</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F263" s="6"/>
       <c r="G263" s="6" t="s">
@@ -9678,7 +9681,7 @@
         <v>5</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F264" s="6"/>
       <c r="G264" s="6" t="s">
@@ -9700,7 +9703,7 @@
         <v>5</v>
       </c>
       <c r="E265" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F265" s="6"/>
       <c r="G265" s="6" t="s">
@@ -9722,7 +9725,7 @@
         <v>5</v>
       </c>
       <c r="E266" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F266" s="6"/>
       <c r="G266" s="6" t="s">
@@ -9744,7 +9747,7 @@
         <v>5</v>
       </c>
       <c r="E267" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F267" s="6"/>
       <c r="G267" s="6" t="s">
@@ -9766,7 +9769,7 @@
         <v>5</v>
       </c>
       <c r="E268" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F268" s="6"/>
       <c r="G268" s="6" t="s">
@@ -9788,7 +9791,7 @@
         <v>5</v>
       </c>
       <c r="E269" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F269" s="6"/>
       <c r="G269" s="6" t="s">
@@ -9810,7 +9813,7 @@
         <v>5</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F270" s="6"/>
       <c r="G270" s="6" t="s">
@@ -9832,7 +9835,7 @@
         <v>5</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F271" s="6"/>
       <c r="G271" s="6" t="s">
@@ -9854,7 +9857,7 @@
         <v>5</v>
       </c>
       <c r="E272" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F272" s="6"/>
       <c r="G272" s="6" t="s">
@@ -9876,7 +9879,7 @@
         <v>5</v>
       </c>
       <c r="E273" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F273" s="6"/>
       <c r="G273" s="6" t="s">
@@ -9898,7 +9901,7 @@
         <v>5</v>
       </c>
       <c r="E274" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F274" s="6"/>
       <c r="G274" s="6" t="s">
@@ -9920,7 +9923,7 @@
         <v>5</v>
       </c>
       <c r="E275" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F275" s="6"/>
       <c r="G275" s="6" t="s">
@@ -9966,7 +9969,7 @@
         <v>5</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6" t="s">
@@ -10032,7 +10035,7 @@
         <v>5</v>
       </c>
       <c r="E280" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6" t="s">
@@ -10054,7 +10057,7 @@
         <v>5</v>
       </c>
       <c r="E281" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F281" s="6"/>
       <c r="G281" s="6" t="s">
@@ -10076,7 +10079,7 @@
         <v>5</v>
       </c>
       <c r="E282" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F282" s="6"/>
       <c r="G282" s="6" t="s">
@@ -10098,7 +10101,7 @@
         <v>5</v>
       </c>
       <c r="E283" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="6" t="s">
@@ -10120,7 +10123,7 @@
         <v>5</v>
       </c>
       <c r="E284" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F284" s="6"/>
       <c r="G284" s="6" t="s">
@@ -10142,7 +10145,7 @@
         <v>5</v>
       </c>
       <c r="E285" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="6" t="s">
@@ -10164,7 +10167,7 @@
         <v>5</v>
       </c>
       <c r="E286" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F286" s="6"/>
       <c r="G286" s="6" t="s">
@@ -10186,7 +10189,7 @@
         <v>5</v>
       </c>
       <c r="E287" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F287" s="6"/>
       <c r="G287" s="6" t="s">
@@ -10208,7 +10211,7 @@
         <v>5</v>
       </c>
       <c r="E288" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F288" s="6"/>
       <c r="G288" s="6" t="s">
@@ -10230,7 +10233,7 @@
         <v>5</v>
       </c>
       <c r="E289" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F289" s="6"/>
       <c r="G289" s="6" t="s">
@@ -10252,7 +10255,7 @@
         <v>5</v>
       </c>
       <c r="E290" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F290" s="6"/>
       <c r="G290" s="6" t="s">
@@ -10274,7 +10277,7 @@
         <v>5</v>
       </c>
       <c r="E291" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F291" s="6"/>
       <c r="G291" s="6" t="s">
@@ -10296,7 +10299,7 @@
         <v>5</v>
       </c>
       <c r="E292" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F292" s="6"/>
       <c r="G292" s="6" t="s">
@@ -10318,7 +10321,7 @@
         <v>5</v>
       </c>
       <c r="E293" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F293" s="6"/>
       <c r="G293" s="6" t="s">
@@ -10340,7 +10343,7 @@
         <v>5</v>
       </c>
       <c r="E294" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F294" s="6"/>
       <c r="G294" s="6" t="s">
@@ -10362,7 +10365,7 @@
         <v>5</v>
       </c>
       <c r="E295" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F295" s="6"/>
       <c r="G295" s="6" t="s">
@@ -10384,7 +10387,7 @@
         <v>5</v>
       </c>
       <c r="E296" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F296" s="6"/>
       <c r="G296" s="6" t="s">
@@ -10406,7 +10409,7 @@
         <v>5</v>
       </c>
       <c r="E297" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F297" s="6"/>
       <c r="G297" s="6" t="s">
@@ -10428,7 +10431,7 @@
         <v>5</v>
       </c>
       <c r="E298" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F298" s="6"/>
       <c r="G298" s="6" t="s">
@@ -10450,7 +10453,7 @@
         <v>5</v>
       </c>
       <c r="E299" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F299" s="6"/>
       <c r="G299" s="6" t="s">
@@ -10472,7 +10475,7 @@
         <v>5</v>
       </c>
       <c r="E300" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F300" s="6"/>
       <c r="G300" s="6" t="s">
@@ -10494,7 +10497,7 @@
         <v>5</v>
       </c>
       <c r="E301" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F301" s="6"/>
       <c r="G301" s="6" t="s">
@@ -10516,7 +10519,7 @@
         <v>5</v>
       </c>
       <c r="E302" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F302" s="6"/>
       <c r="G302" s="6" t="s">
@@ -10538,7 +10541,7 @@
         <v>5</v>
       </c>
       <c r="E303" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F303" s="6"/>
       <c r="G303" s="6" t="s">
@@ -10560,7 +10563,7 @@
         <v>5</v>
       </c>
       <c r="E304" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F304" s="6"/>
       <c r="G304" s="6" t="s">
@@ -10582,7 +10585,7 @@
         <v>5</v>
       </c>
       <c r="E305" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F305" s="6"/>
       <c r="G305" s="6" t="s">
@@ -10604,7 +10607,7 @@
         <v>5</v>
       </c>
       <c r="E306" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F306" s="6"/>
       <c r="G306" s="6" t="s">
@@ -10626,7 +10629,7 @@
         <v>5</v>
       </c>
       <c r="E307" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F307" s="6"/>
       <c r="G307" s="6" t="s">
@@ -10648,7 +10651,7 @@
         <v>5</v>
       </c>
       <c r="E308" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F308" s="6"/>
       <c r="G308" s="6" t="s">
@@ -10670,7 +10673,7 @@
         <v>5</v>
       </c>
       <c r="E309" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F309" s="6"/>
       <c r="G309" s="6" t="s">
@@ -10692,7 +10695,7 @@
         <v>5</v>
       </c>
       <c r="E310" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F310" s="6"/>
       <c r="G310" s="6" t="s">
@@ -10714,7 +10717,7 @@
         <v>5</v>
       </c>
       <c r="E311" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F311" s="6"/>
       <c r="G311" s="6" t="s">
@@ -10736,7 +10739,7 @@
         <v>5</v>
       </c>
       <c r="E312" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F312" s="6"/>
       <c r="G312" s="6" t="s">
@@ -10758,7 +10761,7 @@
         <v>5</v>
       </c>
       <c r="E313" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F313" s="6"/>
       <c r="G313" s="6" t="s">
@@ -10780,7 +10783,7 @@
         <v>5</v>
       </c>
       <c r="E314" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F314" s="6"/>
       <c r="G314" s="6" t="s">
@@ -10824,7 +10827,7 @@
         <v>5</v>
       </c>
       <c r="E316" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F316" s="6"/>
       <c r="G316" s="6" t="s">
@@ -10846,7 +10849,7 @@
         <v>5</v>
       </c>
       <c r="E317" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F317" s="6"/>
       <c r="G317" s="6" t="s">
@@ -10868,7 +10871,7 @@
         <v>5</v>
       </c>
       <c r="E318" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F318" s="6"/>
       <c r="G318" s="6" t="s">
@@ -10890,7 +10893,7 @@
         <v>5</v>
       </c>
       <c r="E319" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F319" s="6"/>
       <c r="G319" s="6" t="s">
@@ -10912,7 +10915,7 @@
         <v>5</v>
       </c>
       <c r="E320" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F320" s="6"/>
       <c r="G320" s="6" t="s">
@@ -12980,7 +12983,7 @@
         <v>5</v>
       </c>
       <c r="E414" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F414" s="6"/>
       <c r="G414" s="6" t="s">
@@ -13002,7 +13005,7 @@
         <v>5</v>
       </c>
       <c r="E415" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F415" s="6"/>
       <c r="G415" s="6" t="s">
@@ -13024,7 +13027,7 @@
         <v>5</v>
       </c>
       <c r="E416" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F416" s="6"/>
       <c r="G416" s="6" t="s">
@@ -13046,7 +13049,7 @@
         <v>5</v>
       </c>
       <c r="E417" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F417" s="6"/>
       <c r="G417" s="6" t="s">
@@ -13068,7 +13071,7 @@
         <v>5</v>
       </c>
       <c r="E418" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F418" s="6"/>
       <c r="G418" s="6" t="s">
@@ -13090,7 +13093,7 @@
         <v>5</v>
       </c>
       <c r="E419" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F419" s="6"/>
       <c r="G419" s="6" t="s">
@@ -13112,7 +13115,7 @@
         <v>5</v>
       </c>
       <c r="E420" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F420" s="6"/>
       <c r="G420" s="6" t="s">
@@ -13134,7 +13137,7 @@
         <v>5</v>
       </c>
       <c r="E421" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F421" s="6"/>
       <c r="G421" s="6" t="s">
@@ -13156,7 +13159,7 @@
         <v>5</v>
       </c>
       <c r="E422" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F422" s="6"/>
       <c r="G422" s="6" t="s">
@@ -13178,7 +13181,7 @@
         <v>5</v>
       </c>
       <c r="E423" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F423" s="6"/>
       <c r="G423" s="6" t="s">
@@ -13200,7 +13203,7 @@
         <v>5</v>
       </c>
       <c r="E424" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F424" s="6"/>
       <c r="G424" s="6" t="s">
@@ -13222,7 +13225,7 @@
         <v>5</v>
       </c>
       <c r="E425" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F425" s="6"/>
       <c r="G425" s="6" t="s">
@@ -13244,7 +13247,7 @@
         <v>5</v>
       </c>
       <c r="E426" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F426" s="6"/>
       <c r="G426" s="6" t="s">
@@ -13266,7 +13269,7 @@
         <v>5</v>
       </c>
       <c r="E427" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F427" s="6"/>
       <c r="G427" s="6" t="s">
@@ -13288,7 +13291,7 @@
         <v>5</v>
       </c>
       <c r="E428" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F428" s="6"/>
       <c r="G428" s="6" t="s">
@@ -13310,7 +13313,7 @@
         <v>5</v>
       </c>
       <c r="E429" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F429" s="6"/>
       <c r="G429" s="6" t="s">
@@ -13332,7 +13335,7 @@
         <v>5</v>
       </c>
       <c r="E430" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F430" s="6"/>
       <c r="G430" s="6" t="s">
@@ -13354,7 +13357,7 @@
         <v>5</v>
       </c>
       <c r="E431" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F431" s="6"/>
       <c r="G431" s="6" t="s">
@@ -13376,7 +13379,7 @@
         <v>5</v>
       </c>
       <c r="E432" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F432" s="6"/>
       <c r="G432" s="6" t="s">
@@ -13398,7 +13401,7 @@
         <v>5</v>
       </c>
       <c r="E433" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F433" s="6"/>
       <c r="G433" s="6" t="s">
@@ -13420,7 +13423,7 @@
         <v>5</v>
       </c>
       <c r="E434" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F434" s="6"/>
       <c r="G434" s="6" t="s">
@@ -13442,7 +13445,7 @@
         <v>5</v>
       </c>
       <c r="E435" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F435" s="6"/>
       <c r="G435" s="6" t="s">
@@ -13464,7 +13467,7 @@
         <v>5</v>
       </c>
       <c r="E436" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F436" s="6"/>
       <c r="G436" s="6" t="s">
@@ -13486,7 +13489,7 @@
         <v>5</v>
       </c>
       <c r="E437" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F437" s="6"/>
       <c r="G437" s="6" t="s">
@@ -13508,7 +13511,7 @@
         <v>5</v>
       </c>
       <c r="E438" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F438" s="6"/>
       <c r="G438" s="6" t="s">
@@ -13530,7 +13533,7 @@
         <v>5</v>
       </c>
       <c r="E439" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F439" s="6"/>
       <c r="G439" s="6" t="s">
@@ -13552,7 +13555,7 @@
         <v>5</v>
       </c>
       <c r="E440" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F440" s="6"/>
       <c r="G440" s="6" t="s">
@@ -13574,7 +13577,7 @@
         <v>5</v>
       </c>
       <c r="E441" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F441" s="6"/>
       <c r="G441" s="6" t="s">
@@ -13596,7 +13599,7 @@
         <v>5</v>
       </c>
       <c r="E442" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F442" s="6"/>
       <c r="G442" s="6" t="s">
@@ -13618,7 +13621,7 @@
         <v>5</v>
       </c>
       <c r="E443" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F443" s="6"/>
       <c r="G443" s="6" t="s">
@@ -13948,7 +13951,7 @@
         <v>5</v>
       </c>
       <c r="E458" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F458" s="6"/>
       <c r="G458" s="6" t="s">
@@ -15048,7 +15051,7 @@
         <v>5</v>
       </c>
       <c r="E508" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F508" s="6"/>
       <c r="G508" s="6" t="s">
@@ -15070,7 +15073,7 @@
         <v>5</v>
       </c>
       <c r="E509" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F509" s="6"/>
       <c r="G509" s="6" t="s">
@@ -15092,7 +15095,7 @@
         <v>5</v>
       </c>
       <c r="E510" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F510" s="6"/>
       <c r="G510" s="6" t="s">
@@ -15114,7 +15117,7 @@
         <v>5</v>
       </c>
       <c r="E511" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F511" s="6"/>
       <c r="G511" s="6" t="s">
@@ -15136,7 +15139,7 @@
         <v>5</v>
       </c>
       <c r="E512" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F512" s="6"/>
       <c r="G512" s="6" t="s">
@@ -15158,7 +15161,7 @@
         <v>5</v>
       </c>
       <c r="E513" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F513" s="6"/>
       <c r="G513" s="6" t="s">
@@ -15180,7 +15183,7 @@
         <v>5</v>
       </c>
       <c r="E514" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F514" s="6"/>
       <c r="G514" s="6" t="s">
@@ -15202,7 +15205,7 @@
         <v>5</v>
       </c>
       <c r="E515" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F515" s="6"/>
       <c r="G515" s="6" t="s">
@@ -15224,7 +15227,7 @@
         <v>5</v>
       </c>
       <c r="E516" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F516" s="6"/>
       <c r="G516" s="6" t="s">
@@ -15246,7 +15249,7 @@
         <v>5</v>
       </c>
       <c r="E517" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F517" s="6"/>
       <c r="G517" s="6" t="s">
@@ -15268,7 +15271,7 @@
         <v>5</v>
       </c>
       <c r="E518" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F518" s="6"/>
       <c r="G518" s="6" t="s">
@@ -15290,7 +15293,7 @@
         <v>5</v>
       </c>
       <c r="E519" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F519" s="6"/>
       <c r="G519" s="6" t="s">
@@ -15312,7 +15315,7 @@
         <v>5</v>
       </c>
       <c r="E520" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F520" s="6"/>
       <c r="G520" s="6" t="s">
@@ -15334,7 +15337,7 @@
         <v>5</v>
       </c>
       <c r="E521" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F521" s="6"/>
       <c r="G521" s="6" t="s">
@@ -15356,7 +15359,7 @@
         <v>5</v>
       </c>
       <c r="E522" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F522" s="6"/>
       <c r="G522" s="6" t="s">
@@ -15378,7 +15381,7 @@
         <v>5</v>
       </c>
       <c r="E523" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F523" s="6"/>
       <c r="G523" s="6" t="s">
@@ -15400,7 +15403,7 @@
         <v>5</v>
       </c>
       <c r="E524" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F524" s="6"/>
       <c r="G524" s="6" t="s">
@@ -15422,7 +15425,7 @@
         <v>5</v>
       </c>
       <c r="E525" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F525" s="6"/>
       <c r="G525" s="6" t="s">
@@ -15444,7 +15447,7 @@
         <v>5</v>
       </c>
       <c r="E526" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F526" s="6"/>
       <c r="G526" s="6" t="s">
@@ -15466,7 +15469,7 @@
         <v>5</v>
       </c>
       <c r="E527" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F527" s="6"/>
       <c r="G527" s="6" t="s">
@@ -15488,7 +15491,7 @@
         <v>5</v>
       </c>
       <c r="E528" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F528" s="6"/>
       <c r="G528" s="6" t="s">
@@ -15510,7 +15513,7 @@
         <v>5</v>
       </c>
       <c r="E529" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F529" s="6"/>
       <c r="G529" s="6" t="s">
@@ -15532,7 +15535,7 @@
         <v>5</v>
       </c>
       <c r="E530" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F530" s="6"/>
       <c r="G530" s="6" t="s">
@@ -15554,7 +15557,7 @@
         <v>5</v>
       </c>
       <c r="E531" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F531" s="6"/>
       <c r="G531" s="6" t="s">
@@ -15576,7 +15579,7 @@
         <v>5</v>
       </c>
       <c r="E532" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F532" s="6"/>
       <c r="G532" s="6" t="s">
@@ -15598,7 +15601,7 @@
         <v>5</v>
       </c>
       <c r="E533" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F533" s="6"/>
       <c r="G533" s="6" t="s">
@@ -15620,7 +15623,7 @@
         <v>5</v>
       </c>
       <c r="E534" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F534" s="6"/>
       <c r="G534" s="6" t="s">
@@ -15642,7 +15645,7 @@
         <v>5</v>
       </c>
       <c r="E535" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F535" s="6"/>
       <c r="G535" s="6" t="s">
@@ -15664,7 +15667,7 @@
         <v>5</v>
       </c>
       <c r="E536" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F536" s="6"/>
       <c r="G536" s="6" t="s">
@@ -15686,7 +15689,7 @@
         <v>5</v>
       </c>
       <c r="E537" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F537" s="6"/>
       <c r="G537" s="6" t="s">
@@ -15708,7 +15711,7 @@
         <v>5</v>
       </c>
       <c r="E538" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F538" s="6"/>
       <c r="G538" s="6" t="s">
@@ -15730,7 +15733,7 @@
         <v>5</v>
       </c>
       <c r="E539" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F539" s="6"/>
       <c r="G539" s="6" t="s">
@@ -15752,7 +15755,7 @@
         <v>5</v>
       </c>
       <c r="E540" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F540" s="6"/>
       <c r="G540" s="6" t="s">
@@ -15818,7 +15821,7 @@
         <v>5</v>
       </c>
       <c r="E543" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F543" s="6"/>
       <c r="G543" s="6" t="s">
@@ -15840,7 +15843,7 @@
         <v>5</v>
       </c>
       <c r="E544" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F544" s="6"/>
       <c r="G544" s="6" t="s">
@@ -15862,7 +15865,7 @@
         <v>5</v>
       </c>
       <c r="E545" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F545" s="6"/>
       <c r="G545" s="6" t="s">
@@ -15884,7 +15887,7 @@
         <v>5</v>
       </c>
       <c r="E546" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F546" s="6"/>
       <c r="G546" s="6" t="s">
@@ -15906,7 +15909,7 @@
         <v>5</v>
       </c>
       <c r="E547" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F547" s="6"/>
       <c r="G547" s="6" t="s">
@@ -15928,7 +15931,7 @@
         <v>5</v>
       </c>
       <c r="E548" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F548" s="6"/>
       <c r="G548" s="6" t="s">
@@ -15950,7 +15953,7 @@
         <v>5</v>
       </c>
       <c r="E549" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F549" s="6"/>
       <c r="G549" s="6" t="s">
@@ -15972,7 +15975,7 @@
         <v>5</v>
       </c>
       <c r="E550" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F550" s="6"/>
       <c r="G550" s="6" t="s">
@@ -15994,7 +15997,7 @@
         <v>5</v>
       </c>
       <c r="E551" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F551" s="6"/>
       <c r="G551" s="6" t="s">
@@ -16016,7 +16019,7 @@
         <v>5</v>
       </c>
       <c r="E552" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F552" s="6"/>
       <c r="G552" s="6" t="s">
@@ -16038,7 +16041,7 @@
         <v>5</v>
       </c>
       <c r="E553" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F553" s="6"/>
       <c r="G553" s="6" t="s">
@@ -16060,7 +16063,7 @@
         <v>5</v>
       </c>
       <c r="E554" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F554" s="6"/>
       <c r="G554" s="6" t="s">
@@ -16082,7 +16085,7 @@
         <v>5</v>
       </c>
       <c r="E555" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F555" s="6"/>
       <c r="G555" s="6" t="s">
@@ -16104,7 +16107,7 @@
         <v>5</v>
       </c>
       <c r="E556" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F556" s="6"/>
       <c r="G556" s="6" t="s">
@@ -16126,7 +16129,7 @@
         <v>5</v>
       </c>
       <c r="E557" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F557" s="6"/>
       <c r="G557" s="6" t="s">
@@ -16148,7 +16151,7 @@
         <v>5</v>
       </c>
       <c r="E558" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F558" s="6"/>
       <c r="G558" s="6" t="s">
@@ -16170,7 +16173,7 @@
         <v>5</v>
       </c>
       <c r="E559" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F559" s="6"/>
       <c r="G559" s="6" t="s">
@@ -16192,7 +16195,7 @@
         <v>5</v>
       </c>
       <c r="E560" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F560" s="6"/>
       <c r="G560" s="6" t="s">
@@ -16214,7 +16217,7 @@
         <v>5</v>
       </c>
       <c r="E561" s="6" t="s">
-        <v>1105</v>
+        <v>1118</v>
       </c>
       <c r="F561" s="6"/>
       <c r="G561" s="6" t="s">
@@ -16940,7 +16943,7 @@
         <v>4</v>
       </c>
       <c r="E594" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F594" s="6"/>
       <c r="G594" s="6" t="s">
@@ -17512,7 +17515,7 @@
         <v>5</v>
       </c>
       <c r="E620" s="6" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="F620" s="6"/>
       <c r="G620" s="6" t="s">
@@ -17842,7 +17845,7 @@
         <v>4</v>
       </c>
       <c r="E635" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F635" s="6"/>
       <c r="G635" s="6" t="s">
@@ -17864,7 +17867,7 @@
         <v>4</v>
       </c>
       <c r="E636" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F636" s="6"/>
       <c r="G636" s="6" t="s">
@@ -17886,7 +17889,7 @@
         <v>4</v>
       </c>
       <c r="E637" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F637" s="6"/>
       <c r="G637" s="6" t="s">
@@ -17908,7 +17911,7 @@
         <v>4</v>
       </c>
       <c r="E638" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F638" s="6"/>
       <c r="G638" s="6" t="s">
@@ -17930,7 +17933,7 @@
         <v>4</v>
       </c>
       <c r="E639" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F639" s="6"/>
       <c r="G639" s="6" t="s">
@@ -17952,7 +17955,7 @@
         <v>4</v>
       </c>
       <c r="E640" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F640" s="6"/>
       <c r="G640" s="6" t="s">
@@ -17974,7 +17977,7 @@
         <v>4</v>
       </c>
       <c r="E641" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F641" s="6"/>
       <c r="G641" s="6" t="s">
@@ -18062,7 +18065,7 @@
         <v>4</v>
       </c>
       <c r="E645" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F645" s="6"/>
       <c r="G645" s="6" t="s">
@@ -18084,7 +18087,7 @@
         <v>4</v>
       </c>
       <c r="E646" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F646" s="6"/>
       <c r="G646" s="6" t="s">
@@ -18106,7 +18109,7 @@
         <v>4</v>
       </c>
       <c r="E647" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F647" s="6"/>
       <c r="G647" s="6" t="s">
@@ -18128,7 +18131,7 @@
         <v>4</v>
       </c>
       <c r="E648" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F648" s="6"/>
       <c r="G648" s="6" t="s">
@@ -18150,7 +18153,7 @@
         <v>4</v>
       </c>
       <c r="E649" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F649" s="6"/>
       <c r="G649" s="6" t="s">
@@ -18172,7 +18175,7 @@
         <v>4</v>
       </c>
       <c r="E650" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F650" s="6"/>
       <c r="G650" s="6" t="s">
@@ -18194,7 +18197,7 @@
         <v>4</v>
       </c>
       <c r="E651" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F651" s="6"/>
       <c r="G651" s="6" t="s">
@@ -18216,7 +18219,7 @@
         <v>4</v>
       </c>
       <c r="E652" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F652" s="6"/>
       <c r="G652" s="6" t="s">
@@ -18238,7 +18241,7 @@
         <v>4</v>
       </c>
       <c r="E653" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F653" s="6"/>
       <c r="G653" s="6" t="s">
@@ -18260,7 +18263,7 @@
         <v>4</v>
       </c>
       <c r="E654" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F654" s="6"/>
       <c r="G654" s="6" t="s">
@@ -18282,7 +18285,7 @@
         <v>4</v>
       </c>
       <c r="E655" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F655" s="6"/>
       <c r="G655" s="6" t="s">
@@ -18304,7 +18307,7 @@
         <v>4</v>
       </c>
       <c r="E656" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F656" s="6"/>
       <c r="G656" s="6" t="s">
@@ -18326,7 +18329,7 @@
         <v>4</v>
       </c>
       <c r="E657" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F657" s="6"/>
       <c r="G657" s="6" t="s">
@@ -18348,7 +18351,7 @@
         <v>4</v>
       </c>
       <c r="E658" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F658" s="6"/>
       <c r="G658" s="6" t="s">
@@ -18392,7 +18395,7 @@
         <v>4</v>
       </c>
       <c r="E660" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F660" s="6"/>
       <c r="G660" s="6" t="s">
@@ -18414,7 +18417,7 @@
         <v>4</v>
       </c>
       <c r="E661" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F661" s="6"/>
       <c r="G661" s="6" t="s">
@@ -18436,7 +18439,7 @@
         <v>4</v>
       </c>
       <c r="E662" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F662" s="6"/>
       <c r="G662" s="6" t="s">
@@ -18458,7 +18461,7 @@
         <v>4</v>
       </c>
       <c r="E663" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F663" s="6"/>
       <c r="G663" s="6" t="s">
@@ -18480,7 +18483,7 @@
         <v>4</v>
       </c>
       <c r="E664" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F664" s="6"/>
       <c r="G664" s="6" t="s">
@@ -18502,7 +18505,7 @@
         <v>4</v>
       </c>
       <c r="E665" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F665" s="6"/>
       <c r="G665" s="6" t="s">
@@ -18546,7 +18549,7 @@
         <v>4</v>
       </c>
       <c r="E667" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F667" s="6"/>
       <c r="G667" s="6" t="s">
@@ -18568,7 +18571,7 @@
         <v>4</v>
       </c>
       <c r="E668" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F668" s="6"/>
       <c r="G668" s="6" t="s">
@@ -18590,7 +18593,7 @@
         <v>4</v>
       </c>
       <c r="E669" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F669" s="6"/>
       <c r="G669" s="6" t="s">
@@ -18612,7 +18615,7 @@
         <v>4</v>
       </c>
       <c r="E670" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F670" s="6"/>
       <c r="G670" s="6" t="s">
@@ -18634,7 +18637,7 @@
         <v>4</v>
       </c>
       <c r="E671" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F671" s="6"/>
       <c r="G671" s="6" t="s">
@@ -18704,7 +18707,7 @@
         <v>4</v>
       </c>
       <c r="E674" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F674" s="6"/>
       <c r="G674" s="6" t="s">
@@ -18726,7 +18729,7 @@
         <v>4</v>
       </c>
       <c r="E675" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F675" s="6"/>
       <c r="G675" s="6" t="s">
@@ -18748,7 +18751,7 @@
         <v>4</v>
       </c>
       <c r="E676" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F676" s="6"/>
       <c r="G676" s="6" t="s">
@@ -18770,7 +18773,7 @@
         <v>4</v>
       </c>
       <c r="E677" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F677" s="6"/>
       <c r="G677" s="6" t="s">
@@ -18792,7 +18795,7 @@
         <v>4</v>
       </c>
       <c r="E678" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F678" s="6"/>
       <c r="G678" s="6" t="s">
@@ -18814,7 +18817,7 @@
         <v>4</v>
       </c>
       <c r="E679" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F679" s="6"/>
       <c r="G679" s="6" t="s">
@@ -18836,7 +18839,7 @@
         <v>4</v>
       </c>
       <c r="E680" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F680" s="6"/>
       <c r="G680" s="6" t="s">
@@ -18858,7 +18861,7 @@
         <v>4</v>
       </c>
       <c r="E681" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F681" s="6"/>
       <c r="G681" s="6" t="s">
@@ -18880,7 +18883,7 @@
         <v>4</v>
       </c>
       <c r="E682" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F682" s="6"/>
       <c r="G682" s="6" t="s">
@@ -18902,7 +18905,7 @@
         <v>4</v>
       </c>
       <c r="E683" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F683" s="6"/>
       <c r="G683" s="6" t="s">
@@ -18924,7 +18927,7 @@
         <v>4</v>
       </c>
       <c r="E684" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F684" s="6"/>
       <c r="G684" s="6" t="s">
@@ -18946,7 +18949,7 @@
         <v>4</v>
       </c>
       <c r="E685" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F685" s="6"/>
       <c r="G685" s="6" t="s">
@@ -18968,7 +18971,7 @@
         <v>4</v>
       </c>
       <c r="E686" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F686" s="6"/>
       <c r="G686" s="6" t="s">
@@ -18990,7 +18993,7 @@
         <v>4</v>
       </c>
       <c r="E687" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F687" s="6"/>
       <c r="G687" s="6" t="s">
@@ -19012,7 +19015,7 @@
         <v>4</v>
       </c>
       <c r="E688" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F688" s="6"/>
       <c r="G688" s="6" t="s">
@@ -19034,7 +19037,7 @@
         <v>4</v>
       </c>
       <c r="E689" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F689" s="6"/>
       <c r="G689" s="6" t="s">
@@ -19056,7 +19059,7 @@
         <v>4</v>
       </c>
       <c r="E690" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F690" s="6"/>
       <c r="G690" s="6" t="s">
@@ -19078,7 +19081,7 @@
         <v>4</v>
       </c>
       <c r="E691" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F691" s="6"/>
       <c r="G691" s="6" t="s">
@@ -19100,7 +19103,7 @@
         <v>4</v>
       </c>
       <c r="E692" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F692" s="6"/>
       <c r="G692" s="6" t="s">
@@ -19122,7 +19125,7 @@
         <v>4</v>
       </c>
       <c r="E693" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F693" s="6"/>
       <c r="G693" s="6" t="s">
@@ -19210,7 +19213,7 @@
         <v>4</v>
       </c>
       <c r="E697" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F697" s="6"/>
       <c r="G697" s="6" t="s">
@@ -19232,7 +19235,7 @@
         <v>4</v>
       </c>
       <c r="E698" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F698" s="6"/>
       <c r="G698" s="6" t="s">
@@ -19254,7 +19257,7 @@
         <v>4</v>
       </c>
       <c r="E699" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F699" s="6"/>
       <c r="G699" s="6" t="s">
@@ -19276,7 +19279,7 @@
         <v>4</v>
       </c>
       <c r="E700" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F700" s="6"/>
       <c r="G700" s="6" t="s">
@@ -19346,7 +19349,7 @@
         <v>4</v>
       </c>
       <c r="E703" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F703" s="6"/>
       <c r="G703" s="6" t="s">
@@ -19456,7 +19459,7 @@
         <v>4</v>
       </c>
       <c r="E708" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F708" s="6"/>
       <c r="G708" s="6" t="s">
@@ -19478,7 +19481,7 @@
         <v>4</v>
       </c>
       <c r="E709" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F709" s="6"/>
       <c r="G709" s="6" t="s">
@@ -19500,7 +19503,7 @@
         <v>4</v>
       </c>
       <c r="E710" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F710" s="6"/>
       <c r="G710" s="6" t="s">
@@ -19522,7 +19525,7 @@
         <v>4</v>
       </c>
       <c r="E711" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F711" s="6"/>
       <c r="G711" s="6" t="s">
@@ -19544,7 +19547,7 @@
         <v>4</v>
       </c>
       <c r="E712" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F712" s="6"/>
       <c r="G712" s="6" t="s">
@@ -19566,7 +19569,7 @@
         <v>4</v>
       </c>
       <c r="E713" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F713" s="6"/>
       <c r="G713" s="6" t="s">
@@ -19588,7 +19591,7 @@
         <v>4</v>
       </c>
       <c r="E714" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F714" s="6"/>
       <c r="G714" s="6" t="s">
@@ -19610,7 +19613,7 @@
         <v>4</v>
       </c>
       <c r="E715" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F715" s="6"/>
       <c r="G715" s="6" t="s">
@@ -19632,7 +19635,7 @@
         <v>4</v>
       </c>
       <c r="E716" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F716" s="6"/>
       <c r="G716" s="6" t="s">
@@ -19654,7 +19657,7 @@
         <v>4</v>
       </c>
       <c r="E717" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F717" s="6"/>
       <c r="G717" s="6" t="s">
@@ -19676,7 +19679,7 @@
         <v>4</v>
       </c>
       <c r="E718" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F718" s="6"/>
       <c r="G718" s="6" t="s">
@@ -19698,7 +19701,7 @@
         <v>4</v>
       </c>
       <c r="E719" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F719" s="6"/>
       <c r="G719" s="6" t="s">
@@ -19720,7 +19723,7 @@
         <v>4</v>
       </c>
       <c r="E720" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F720" s="6"/>
       <c r="G720" s="6" t="s">
@@ -19742,7 +19745,7 @@
         <v>4</v>
       </c>
       <c r="E721" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F721" s="6"/>
       <c r="G721" s="6" t="s">
@@ -19764,7 +19767,7 @@
         <v>4</v>
       </c>
       <c r="E722" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F722" s="6"/>
       <c r="G722" s="6" t="s">
@@ -19786,7 +19789,7 @@
         <v>4</v>
       </c>
       <c r="E723" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F723" s="6"/>
       <c r="G723" s="6" t="s">
@@ -19808,7 +19811,7 @@
         <v>4</v>
       </c>
       <c r="E724" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F724" s="6"/>
       <c r="G724" s="6" t="s">
@@ -19830,7 +19833,7 @@
         <v>4</v>
       </c>
       <c r="E725" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F725" s="6"/>
       <c r="G725" s="6" t="s">
@@ -19852,7 +19855,7 @@
         <v>4</v>
       </c>
       <c r="E726" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F726" s="6"/>
       <c r="G726" s="6" t="s">
@@ -19874,7 +19877,7 @@
         <v>4</v>
       </c>
       <c r="E727" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F727" s="6"/>
       <c r="G727" s="6" t="s">
@@ -19896,7 +19899,7 @@
         <v>4</v>
       </c>
       <c r="E728" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F728" s="6"/>
       <c r="G728" s="6" t="s">
@@ -19918,7 +19921,7 @@
         <v>4</v>
       </c>
       <c r="E729" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F729" s="6"/>
       <c r="G729" s="6" t="s">
@@ -19940,7 +19943,7 @@
         <v>4</v>
       </c>
       <c r="E730" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F730" s="6"/>
       <c r="G730" s="6" t="s">
@@ -19962,7 +19965,7 @@
         <v>4</v>
       </c>
       <c r="E731" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F731" s="6"/>
       <c r="G731" s="6" t="s">
@@ -19984,7 +19987,7 @@
         <v>4</v>
       </c>
       <c r="E732" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F732" s="6"/>
       <c r="G732" s="6" t="s">
@@ -20006,7 +20009,7 @@
         <v>4</v>
       </c>
       <c r="E733" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F733" s="6"/>
       <c r="G733" s="6" t="s">
@@ -20028,7 +20031,7 @@
         <v>4</v>
       </c>
       <c r="E734" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F734" s="6"/>
       <c r="G734" s="6" t="s">
@@ -20050,7 +20053,7 @@
         <v>4</v>
       </c>
       <c r="E735" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F735" s="6"/>
       <c r="G735" s="6" t="s">
@@ -20072,7 +20075,7 @@
         <v>4</v>
       </c>
       <c r="E736" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F736" s="6"/>
       <c r="G736" s="6" t="s">
@@ -20094,7 +20097,7 @@
         <v>4</v>
       </c>
       <c r="E737" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F737" s="6"/>
       <c r="G737" s="6" t="s">
@@ -20116,7 +20119,7 @@
         <v>4</v>
       </c>
       <c r="E738" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F738" s="6"/>
       <c r="G738" s="6" t="s">
@@ -20138,7 +20141,7 @@
         <v>4</v>
       </c>
       <c r="E739" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F739" s="6"/>
       <c r="G739" s="6" t="s">
@@ -20160,7 +20163,7 @@
         <v>4</v>
       </c>
       <c r="E740" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F740" s="6"/>
       <c r="G740" s="6" t="s">
@@ -20182,7 +20185,7 @@
         <v>4</v>
       </c>
       <c r="E741" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F741" s="6"/>
       <c r="G741" s="6" t="s">
@@ -20204,7 +20207,7 @@
         <v>4</v>
       </c>
       <c r="E742" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F742" s="6"/>
       <c r="G742" s="6" t="s">
@@ -20226,7 +20229,7 @@
         <v>4</v>
       </c>
       <c r="E743" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F743" s="6"/>
       <c r="G743" s="6" t="s">
@@ -20248,7 +20251,7 @@
         <v>4</v>
       </c>
       <c r="E744" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F744" s="6"/>
       <c r="G744" s="6" t="s">
@@ -20270,7 +20273,7 @@
         <v>4</v>
       </c>
       <c r="E745" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F745" s="6"/>
       <c r="G745" s="6" t="s">
@@ -20292,7 +20295,7 @@
         <v>4</v>
       </c>
       <c r="E746" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F746" s="6"/>
       <c r="G746" s="6" t="s">
@@ -20314,7 +20317,7 @@
         <v>4</v>
       </c>
       <c r="E747" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F747" s="6"/>
       <c r="G747" s="6" t="s">
@@ -20336,7 +20339,7 @@
         <v>4</v>
       </c>
       <c r="E748" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F748" s="6"/>
       <c r="G748" s="6" t="s">
@@ -20358,7 +20361,7 @@
         <v>4</v>
       </c>
       <c r="E749" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F749" s="6"/>
       <c r="G749" s="6" t="s">
@@ -20380,7 +20383,7 @@
         <v>4</v>
       </c>
       <c r="E750" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F750" s="6"/>
       <c r="G750" s="6" t="s">
@@ -20402,7 +20405,7 @@
         <v>4</v>
       </c>
       <c r="E751" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F751" s="6"/>
       <c r="G751" s="6" t="s">
@@ -20424,7 +20427,7 @@
         <v>4</v>
       </c>
       <c r="E752" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F752" s="6"/>
       <c r="G752" s="6" t="s">
@@ -20446,7 +20449,7 @@
         <v>4</v>
       </c>
       <c r="E753" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F753" s="6"/>
       <c r="G753" s="6" t="s">
@@ -20468,7 +20471,7 @@
         <v>4</v>
       </c>
       <c r="E754" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F754" s="6"/>
       <c r="G754" s="6" t="s">
@@ -20490,7 +20493,7 @@
         <v>4</v>
       </c>
       <c r="E755" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F755" s="6"/>
       <c r="G755" s="6" t="s">
@@ -20512,7 +20515,7 @@
         <v>4</v>
       </c>
       <c r="E756" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F756" s="6"/>
       <c r="G756" s="6" t="s">
@@ -20534,7 +20537,7 @@
         <v>4</v>
       </c>
       <c r="E757" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F757" s="6"/>
       <c r="G757" s="6" t="s">
@@ -20556,7 +20559,7 @@
         <v>4</v>
       </c>
       <c r="E758" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F758" s="6"/>
       <c r="G758" s="6" t="s">
@@ -20578,7 +20581,7 @@
         <v>4</v>
       </c>
       <c r="E759" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F759" s="6"/>
       <c r="G759" s="6" t="s">
@@ -20600,7 +20603,7 @@
         <v>4</v>
       </c>
       <c r="E760" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F760" s="6"/>
       <c r="G760" s="6" t="s">
@@ -20622,7 +20625,7 @@
         <v>4</v>
       </c>
       <c r="E761" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F761" s="6"/>
       <c r="G761" s="6" t="s">
@@ -20644,7 +20647,7 @@
         <v>4</v>
       </c>
       <c r="E762" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F762" s="6"/>
       <c r="G762" s="6" t="s">
@@ -20666,7 +20669,7 @@
         <v>4</v>
       </c>
       <c r="E763" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F763" s="6"/>
       <c r="G763" s="6" t="s">
@@ -20688,7 +20691,7 @@
         <v>4</v>
       </c>
       <c r="E764" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F764" s="6"/>
       <c r="G764" s="6" t="s">
@@ -20710,7 +20713,7 @@
         <v>4</v>
       </c>
       <c r="E765" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F765" s="6"/>
       <c r="G765" s="6" t="s">
@@ -20732,7 +20735,7 @@
         <v>4</v>
       </c>
       <c r="E766" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F766" s="6"/>
       <c r="G766" s="6" t="s">
@@ -20754,7 +20757,7 @@
         <v>4</v>
       </c>
       <c r="E767" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F767" s="6"/>
       <c r="G767" s="6" t="s">
@@ -20776,7 +20779,7 @@
         <v>4</v>
       </c>
       <c r="E768" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F768" s="6"/>
       <c r="G768" s="6" t="s">
@@ -20798,7 +20801,7 @@
         <v>4</v>
       </c>
       <c r="E769" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F769" s="6"/>
       <c r="G769" s="6" t="s">
@@ -20820,7 +20823,7 @@
         <v>4</v>
       </c>
       <c r="E770" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F770" s="6"/>
       <c r="G770" s="6" t="s">
@@ -20842,7 +20845,7 @@
         <v>4</v>
       </c>
       <c r="E771" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F771" s="6"/>
       <c r="G771" s="6" t="s">
@@ -20864,7 +20867,7 @@
         <v>4</v>
       </c>
       <c r="E772" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F772" s="6"/>
       <c r="G772" s="6" t="s">
@@ -20886,7 +20889,7 @@
         <v>4</v>
       </c>
       <c r="E773" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F773" s="6"/>
       <c r="G773" s="6" t="s">
@@ -20908,7 +20911,7 @@
         <v>4</v>
       </c>
       <c r="E774" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F774" s="6"/>
       <c r="G774" s="6" t="s">
@@ -20930,7 +20933,7 @@
         <v>4</v>
       </c>
       <c r="E775" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F775" s="6"/>
       <c r="G775" s="6" t="s">
@@ -20952,7 +20955,7 @@
         <v>4</v>
       </c>
       <c r="E776" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F776" s="6"/>
       <c r="G776" s="6" t="s">
@@ -20974,7 +20977,7 @@
         <v>4</v>
       </c>
       <c r="E777" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F777" s="6"/>
       <c r="G777" s="6" t="s">
@@ -20996,7 +20999,7 @@
         <v>4</v>
       </c>
       <c r="E778" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F778" s="6"/>
       <c r="G778" s="6" t="s">
@@ -21018,7 +21021,7 @@
         <v>4</v>
       </c>
       <c r="E779" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F779" s="6"/>
       <c r="G779" s="6" t="s">
@@ -21040,7 +21043,7 @@
         <v>4</v>
       </c>
       <c r="E780" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F780" s="6"/>
       <c r="G780" s="6" t="s">
@@ -21062,7 +21065,7 @@
         <v>4</v>
       </c>
       <c r="E781" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F781" s="6"/>
       <c r="G781" s="6" t="s">
@@ -21084,7 +21087,7 @@
         <v>4</v>
       </c>
       <c r="E782" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F782" s="6"/>
       <c r="G782" s="6" t="s">
@@ -21106,7 +21109,7 @@
         <v>4</v>
       </c>
       <c r="E783" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F783" s="6"/>
       <c r="G783" s="6" t="s">
@@ -21128,7 +21131,7 @@
         <v>4</v>
       </c>
       <c r="E784" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F784" s="6"/>
       <c r="G784" s="6" t="s">
@@ -21150,7 +21153,7 @@
         <v>4</v>
       </c>
       <c r="E785" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F785" s="6"/>
       <c r="G785" s="6" t="s">
@@ -21172,7 +21175,7 @@
         <v>4</v>
       </c>
       <c r="E786" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F786" s="6"/>
       <c r="G786" s="6" t="s">
@@ -21194,7 +21197,7 @@
         <v>4</v>
       </c>
       <c r="E787" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F787" s="6"/>
       <c r="G787" s="6" t="s">
@@ -21216,7 +21219,7 @@
         <v>4</v>
       </c>
       <c r="E788" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F788" s="6"/>
       <c r="G788" s="6" t="s">
@@ -21238,7 +21241,7 @@
         <v>4</v>
       </c>
       <c r="E789" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F789" s="6"/>
       <c r="G789" s="6" t="s">
@@ -21260,7 +21263,7 @@
         <v>4</v>
       </c>
       <c r="E790" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F790" s="6"/>
       <c r="G790" s="6" t="s">
@@ -21282,7 +21285,7 @@
         <v>4</v>
       </c>
       <c r="E791" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F791" s="6"/>
       <c r="G791" s="6" t="s">
@@ -21304,7 +21307,7 @@
         <v>4</v>
       </c>
       <c r="E792" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F792" s="6"/>
       <c r="G792" s="6" t="s">
@@ -21326,7 +21329,7 @@
         <v>4</v>
       </c>
       <c r="E793" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F793" s="6"/>
       <c r="G793" s="6" t="s">
@@ -21348,7 +21351,7 @@
         <v>4</v>
       </c>
       <c r="E794" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F794" s="6"/>
       <c r="G794" s="6" t="s">
@@ -21370,7 +21373,7 @@
         <v>4</v>
       </c>
       <c r="E795" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F795" s="6"/>
       <c r="G795" s="6" t="s">
@@ -21392,7 +21395,7 @@
         <v>4</v>
       </c>
       <c r="E796" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F796" s="6"/>
       <c r="G796" s="6" t="s">
@@ -21414,7 +21417,7 @@
         <v>4</v>
       </c>
       <c r="E797" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F797" s="6"/>
       <c r="G797" s="6" t="s">
@@ -21436,7 +21439,7 @@
         <v>4</v>
       </c>
       <c r="E798" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F798" s="6"/>
       <c r="G798" s="6" t="s">
@@ -21458,7 +21461,7 @@
         <v>4</v>
       </c>
       <c r="E799" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F799" s="6"/>
       <c r="G799" s="6" t="s">
@@ -21480,7 +21483,7 @@
         <v>4</v>
       </c>
       <c r="E800" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F800" s="6"/>
       <c r="G800" s="6" t="s">
@@ -21502,7 +21505,7 @@
         <v>4</v>
       </c>
       <c r="E801" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F801" s="6"/>
       <c r="G801" s="6" t="s">
@@ -21524,7 +21527,7 @@
         <v>4</v>
       </c>
       <c r="E802" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F802" s="6"/>
       <c r="G802" s="6" t="s">
@@ -21546,7 +21549,7 @@
         <v>4</v>
       </c>
       <c r="E803" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F803" s="6"/>
       <c r="G803" s="6" t="s">
@@ -21568,7 +21571,7 @@
         <v>4</v>
       </c>
       <c r="E804" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F804" s="6"/>
       <c r="G804" s="6" t="s">
@@ -21590,7 +21593,7 @@
         <v>4</v>
       </c>
       <c r="E805" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F805" s="6"/>
       <c r="G805" s="6" t="s">
@@ -21612,7 +21615,7 @@
         <v>4</v>
       </c>
       <c r="E806" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F806" s="6"/>
       <c r="G806" s="6" t="s">
@@ -21634,7 +21637,7 @@
         <v>4</v>
       </c>
       <c r="E807" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F807" s="6"/>
       <c r="G807" s="6" t="s">
@@ -21656,7 +21659,7 @@
         <v>4</v>
       </c>
       <c r="E808" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F808" s="6"/>
       <c r="G808" s="6" t="s">
@@ -21678,7 +21681,7 @@
         <v>4</v>
       </c>
       <c r="E809" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F809" s="6"/>
       <c r="G809" s="6" t="s">
@@ -21700,7 +21703,7 @@
         <v>4</v>
       </c>
       <c r="E810" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F810" s="6"/>
       <c r="G810" s="6" t="s">
@@ -21722,7 +21725,7 @@
         <v>4</v>
       </c>
       <c r="E811" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F811" s="6"/>
       <c r="G811" s="6" t="s">
@@ -21744,7 +21747,7 @@
         <v>4</v>
       </c>
       <c r="E812" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F812" s="6"/>
       <c r="G812" s="6" t="s">
@@ -21766,7 +21769,7 @@
         <v>4</v>
       </c>
       <c r="E813" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F813" s="6"/>
       <c r="G813" s="6" t="s">
@@ -21788,7 +21791,7 @@
         <v>4</v>
       </c>
       <c r="E814" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F814" s="6"/>
       <c r="G814" s="6" t="s">
@@ -21810,7 +21813,7 @@
         <v>4</v>
       </c>
       <c r="E815" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F815" s="6"/>
       <c r="G815" s="6" t="s">
@@ -21832,7 +21835,7 @@
         <v>4</v>
       </c>
       <c r="E816" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F816" s="6"/>
       <c r="G816" s="6" t="s">
@@ -21854,7 +21857,7 @@
         <v>4</v>
       </c>
       <c r="E817" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F817" s="6"/>
       <c r="G817" s="6" t="s">
@@ -21876,7 +21879,7 @@
         <v>4</v>
       </c>
       <c r="E818" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F818" s="6"/>
       <c r="G818" s="6" t="s">
@@ -21898,7 +21901,7 @@
         <v>4</v>
       </c>
       <c r="E819" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F819" s="6"/>
       <c r="G819" s="6" t="s">
@@ -21920,7 +21923,7 @@
         <v>4</v>
       </c>
       <c r="E820" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F820" s="6"/>
       <c r="G820" s="6" t="s">
@@ -21942,7 +21945,7 @@
         <v>4</v>
       </c>
       <c r="E821" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F821" s="6"/>
       <c r="G821" s="6" t="s">
@@ -21964,7 +21967,7 @@
         <v>4</v>
       </c>
       <c r="E822" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F822" s="6"/>
       <c r="G822" s="6" t="s">
@@ -21986,7 +21989,7 @@
         <v>4</v>
       </c>
       <c r="E823" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F823" s="6"/>
       <c r="G823" s="6" t="s">
@@ -22008,7 +22011,7 @@
         <v>4</v>
       </c>
       <c r="E824" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F824" s="6"/>
       <c r="G824" s="6" t="s">
@@ -22030,7 +22033,7 @@
         <v>4</v>
       </c>
       <c r="E825" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F825" s="6"/>
       <c r="G825" s="6" t="s">
@@ -22052,7 +22055,7 @@
         <v>4</v>
       </c>
       <c r="E826" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F826" s="6"/>
       <c r="G826" s="6" t="s">
@@ -22074,7 +22077,7 @@
         <v>4</v>
       </c>
       <c r="E827" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F827" s="6"/>
       <c r="G827" s="6" t="s">
@@ -22096,7 +22099,7 @@
         <v>4</v>
       </c>
       <c r="E828" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F828" s="6"/>
       <c r="G828" s="6" t="s">
@@ -22118,7 +22121,7 @@
         <v>4</v>
       </c>
       <c r="E829" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F829" s="6"/>
       <c r="G829" s="6" t="s">
@@ -22140,7 +22143,7 @@
         <v>4</v>
       </c>
       <c r="E830" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F830" s="6"/>
       <c r="G830" s="6" t="s">
@@ -22162,7 +22165,7 @@
         <v>4</v>
       </c>
       <c r="E831" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F831" s="6"/>
       <c r="G831" s="6" t="s">
@@ -22184,7 +22187,7 @@
         <v>4</v>
       </c>
       <c r="E832" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F832" s="6"/>
       <c r="G832" s="6" t="s">
@@ -22206,7 +22209,7 @@
         <v>4</v>
       </c>
       <c r="E833" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F833" s="6"/>
       <c r="G833" s="6" t="s">
@@ -22228,7 +22231,7 @@
         <v>4</v>
       </c>
       <c r="E834" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F834" s="6"/>
       <c r="G834" s="6" t="s">
@@ -22250,7 +22253,7 @@
         <v>4</v>
       </c>
       <c r="E835" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F835" s="6"/>
       <c r="G835" s="6" t="s">
@@ -22272,7 +22275,7 @@
         <v>4</v>
       </c>
       <c r="E836" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F836" s="6"/>
       <c r="G836" s="6" t="s">
@@ -22294,7 +22297,7 @@
         <v>4</v>
       </c>
       <c r="E837" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F837" s="6"/>
       <c r="G837" s="6" t="s">
@@ -22316,7 +22319,7 @@
         <v>4</v>
       </c>
       <c r="E838" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F838" s="6"/>
       <c r="G838" s="6" t="s">
@@ -22338,7 +22341,7 @@
         <v>4</v>
       </c>
       <c r="E839" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F839" s="6"/>
       <c r="G839" s="6" t="s">
@@ -22360,7 +22363,7 @@
         <v>4</v>
       </c>
       <c r="E840" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F840" s="6"/>
       <c r="G840" s="6" t="s">
@@ -22382,7 +22385,7 @@
         <v>4</v>
       </c>
       <c r="E841" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F841" s="6"/>
       <c r="G841" s="6" t="s">
@@ -22404,7 +22407,7 @@
         <v>4</v>
       </c>
       <c r="E842" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F842" s="6"/>
       <c r="G842" s="6" t="s">
@@ -22426,7 +22429,7 @@
         <v>4</v>
       </c>
       <c r="E843" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F843" s="6"/>
       <c r="G843" s="6" t="s">
@@ -22448,7 +22451,7 @@
         <v>4</v>
       </c>
       <c r="E844" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F844" s="6"/>
       <c r="G844" s="6" t="s">
@@ -22470,7 +22473,7 @@
         <v>4</v>
       </c>
       <c r="E845" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F845" s="6"/>
       <c r="G845" s="6" t="s">
@@ -22492,7 +22495,7 @@
         <v>4</v>
       </c>
       <c r="E846" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F846" s="6"/>
       <c r="G846" s="6" t="s">
@@ -22514,7 +22517,7 @@
         <v>4</v>
       </c>
       <c r="E847" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F847" s="6"/>
       <c r="G847" s="6" t="s">
@@ -22536,7 +22539,7 @@
         <v>4</v>
       </c>
       <c r="E848" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F848" s="6"/>
       <c r="G848" s="6" t="s">
@@ -22558,7 +22561,7 @@
         <v>4</v>
       </c>
       <c r="E849" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F849" s="6"/>
       <c r="G849" s="6" t="s">
@@ -22580,7 +22583,7 @@
         <v>4</v>
       </c>
       <c r="E850" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F850" s="6"/>
       <c r="G850" s="6" t="s">
@@ -22602,7 +22605,7 @@
         <v>4</v>
       </c>
       <c r="E851" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F851" s="6"/>
       <c r="G851" s="6" t="s">
@@ -22624,7 +22627,7 @@
         <v>4</v>
       </c>
       <c r="E852" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F852" s="6"/>
       <c r="G852" s="6" t="s">
@@ -22646,7 +22649,7 @@
         <v>4</v>
       </c>
       <c r="E853" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F853" s="6"/>
       <c r="G853" s="6" t="s">
@@ -22668,7 +22671,7 @@
         <v>4</v>
       </c>
       <c r="E854" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F854" s="6"/>
       <c r="G854" s="6" t="s">
@@ -22690,7 +22693,7 @@
         <v>4</v>
       </c>
       <c r="E855" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F855" s="6"/>
       <c r="G855" s="6" t="s">
@@ -22712,7 +22715,7 @@
         <v>4</v>
       </c>
       <c r="E856" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F856" s="6"/>
       <c r="G856" s="6" t="s">
@@ -22734,7 +22737,7 @@
         <v>4</v>
       </c>
       <c r="E857" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F857" s="6"/>
       <c r="G857" s="6" t="s">
@@ -22756,7 +22759,7 @@
         <v>4</v>
       </c>
       <c r="E858" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F858" s="6"/>
       <c r="G858" s="6" t="s">
@@ -22778,7 +22781,7 @@
         <v>4</v>
       </c>
       <c r="E859" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F859" s="6"/>
       <c r="G859" s="6" t="s">
@@ -23196,7 +23199,7 @@
         <v>4</v>
       </c>
       <c r="E878" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F878" s="6"/>
       <c r="G878" s="6" t="s">
@@ -23306,7 +23309,7 @@
         <v>4</v>
       </c>
       <c r="E883" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="F883" s="6"/>
       <c r="G883" s="6" t="s">
@@ -23438,7 +23441,7 @@
         <v>5</v>
       </c>
       <c r="E889" s="6" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F889" s="6"/>
       <c r="G889" s="6" t="s">
@@ -23616,7 +23619,7 @@
         <v>5</v>
       </c>
       <c r="E897" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F897" s="6"/>
       <c r="G897" s="6" t="s">
@@ -23638,7 +23641,7 @@
         <v>5</v>
       </c>
       <c r="E898" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F898" s="6"/>
       <c r="G898" s="6" t="s">
@@ -23660,7 +23663,7 @@
         <v>5</v>
       </c>
       <c r="E899" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F899" s="6"/>
       <c r="G899" s="6" t="s">
@@ -23706,7 +23709,7 @@
         <v>5</v>
       </c>
       <c r="E901" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F901" s="6"/>
       <c r="G901" s="6" t="s">
@@ -23728,7 +23731,7 @@
         <v>5</v>
       </c>
       <c r="E902" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F902" s="6"/>
       <c r="G902" s="6" t="s">
@@ -23750,7 +23753,7 @@
         <v>5</v>
       </c>
       <c r="E903" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F903" s="6"/>
       <c r="G903" s="6" t="s">
@@ -24740,7 +24743,7 @@
         <v>5</v>
       </c>
       <c r="E948" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F948" s="6"/>
       <c r="G948" s="6" t="s">
@@ -24762,7 +24765,7 @@
         <v>5</v>
       </c>
       <c r="E949" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F949" s="6"/>
       <c r="G949" s="6" t="s">
@@ -24784,7 +24787,7 @@
         <v>5</v>
       </c>
       <c r="E950" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F950" s="6"/>
       <c r="G950" s="6" t="s">
@@ -25334,7 +25337,7 @@
         <v>5</v>
       </c>
       <c r="E975" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F975" s="6"/>
       <c r="G975" s="6" t="s">
@@ -25356,7 +25359,7 @@
         <v>5</v>
       </c>
       <c r="E976" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F976" s="6"/>
       <c r="G976" s="6" t="s">
@@ -25378,7 +25381,7 @@
         <v>5</v>
       </c>
       <c r="E977" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F977" s="6"/>
       <c r="G977" s="6" t="s">
@@ -25400,7 +25403,7 @@
         <v>5</v>
       </c>
       <c r="E978" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F978" s="6"/>
       <c r="G978" s="6" t="s">
@@ -25422,7 +25425,7 @@
         <v>5</v>
       </c>
       <c r="E979" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F979" s="6"/>
       <c r="G979" s="6" t="s">
@@ -25444,7 +25447,7 @@
         <v>5</v>
       </c>
       <c r="E980" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F980" s="6"/>
       <c r="G980" s="6" t="s">
@@ -25466,7 +25469,7 @@
         <v>5</v>
       </c>
       <c r="E981" s="6" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F981" s="6"/>
       <c r="G981" s="6" t="s">
@@ -25774,7 +25777,7 @@
         <v>5</v>
       </c>
       <c r="E995" s="6" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F995" s="6"/>
       <c r="G995" s="6" t="s">
@@ -25798,7 +25801,7 @@
         <v>5</v>
       </c>
       <c r="E996" s="6" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F996" s="6"/>
       <c r="G996" s="6" t="s">
@@ -25822,7 +25825,7 @@
         <v>4</v>
       </c>
       <c r="E997" s="6" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F997" s="6"/>
       <c r="G997" s="6" t="s">
@@ -25844,7 +25847,7 @@
         <v>4</v>
       </c>
       <c r="E998" s="6" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F998" s="6"/>
       <c r="G998" s="6" t="s">

</xml_diff>

<commit_message>
se actualizo la area con las en abse a las tablasweb_ltl
wcross_dock
etransferencia_trading
etrans_detalle_cross_dock
web_lots
web_tracking_stage
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes activos.xlsx
+++ b/00-Documentacion/Listado de reportes activos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55066F12-D5D2-4DE9-B0FF-601B9A7BFEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7DDF12-593A-421F-9D4B-8772C67BE037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="1815" windowWidth="15375" windowHeight="7875" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="1122">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -3401,6 +3401,9 @@
   </si>
   <si>
     <t>pdf,zip,correo,excel,xml</t>
+  </si>
+  <si>
+    <t>excel,correo,pdf, ws</t>
   </si>
 </sst>
 </file>
@@ -3504,7 +3507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3524,6 +3527,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3842,7 +3846,7 @@
   <dimension ref="A1:H1007"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F902" sqref="F902:G902"/>
+      <selection activeCell="F1012" sqref="F1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10795,7 +10799,7 @@
       </c>
       <c r="H314" s="6"/>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="6">
         <v>39</v>
       </c>
@@ -10809,7 +10813,7 @@
         <v>4</v>
       </c>
       <c r="E315" s="6" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="F315" s="6"/>
       <c r="G315" s="6" t="s">
@@ -16352,8 +16356,8 @@
       <c r="D567" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E567" s="6" t="s">
-        <v>1108</v>
+      <c r="E567" s="7" t="s">
+        <v>1121</v>
       </c>
       <c r="F567" s="6"/>
       <c r="G567" s="6" t="s">
@@ -16374,8 +16378,8 @@
       <c r="D568" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E568" s="6" t="s">
-        <v>1108</v>
+      <c r="E568" s="7" t="s">
+        <v>1121</v>
       </c>
       <c r="F568" s="6"/>
       <c r="G568" s="6" t="s">
@@ -16396,8 +16400,8 @@
       <c r="D569" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E569" s="6" t="s">
-        <v>1108</v>
+      <c r="E569" s="7" t="s">
+        <v>1121</v>
       </c>
       <c r="F569" s="6"/>
       <c r="G569" s="6" t="s">
@@ -19181,7 +19185,7 @@
       </c>
       <c r="H695" s="6"/>
     </row>
-    <row r="696" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A696" s="6">
         <v>39</v>
       </c>
@@ -19195,7 +19199,7 @@
         <v>4</v>
       </c>
       <c r="E696" s="6" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="F696" s="6"/>
       <c r="G696" s="6" t="s">
@@ -23477,7 +23481,7 @@
       </c>
       <c r="H890" s="6"/>
     </row>
-    <row r="891" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A891" s="6">
         <v>39</v>
       </c>
@@ -23491,7 +23495,7 @@
         <v>4</v>
       </c>
       <c r="E891" s="6" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="F891" s="6"/>
       <c r="G891" s="6" t="s">
@@ -23565,7 +23569,7 @@
       </c>
       <c r="H894" s="6"/>
     </row>
-    <row r="895" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A895" s="6">
         <v>39</v>
       </c>
@@ -23579,7 +23583,7 @@
         <v>4</v>
       </c>
       <c r="E895" s="6" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="F895" s="6"/>
       <c r="G895" s="6" t="s">
@@ -23587,7 +23591,7 @@
       </c>
       <c r="H895" s="6"/>
     </row>
-    <row r="896" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A896" s="6">
         <v>39</v>
       </c>
@@ -23601,7 +23605,7 @@
         <v>4</v>
       </c>
       <c r="E896" s="6" t="s">
-        <v>1085</v>
+        <v>1101</v>
       </c>
       <c r="F896" s="6"/>
       <c r="G896" s="6" t="s">
@@ -23609,7 +23613,7 @@
       </c>
       <c r="H896" s="6"/>
     </row>
-    <row r="897" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A897" s="6">
         <v>80</v>
       </c>
@@ -23631,7 +23635,7 @@
       </c>
       <c r="H897" s="6"/>
     </row>
-    <row r="898" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898" s="6">
         <v>80</v>
       </c>
@@ -23653,7 +23657,7 @@
       </c>
       <c r="H898" s="6"/>
     </row>
-    <row r="899" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A899" s="6">
         <v>80</v>
       </c>
@@ -23699,7 +23703,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="901" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A901" s="6">
         <v>80</v>
       </c>
@@ -23721,7 +23725,7 @@
       </c>
       <c r="H901" s="6"/>
     </row>
-    <row r="902" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" s="6">
         <v>80</v>
       </c>
@@ -23743,7 +23747,7 @@
       </c>
       <c r="H902" s="6"/>
     </row>
-    <row r="903" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A903" s="6">
         <v>80</v>
       </c>
@@ -24733,7 +24737,7 @@
       </c>
       <c r="H947" s="6"/>
     </row>
-    <row r="948" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A948" s="6">
         <v>80</v>
       </c>
@@ -24755,7 +24759,7 @@
       </c>
       <c r="H948" s="6"/>
     </row>
-    <row r="949" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A949" s="6">
         <v>80</v>
       </c>
@@ -24777,7 +24781,7 @@
       </c>
       <c r="H949" s="6"/>
     </row>
-    <row r="950" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A950" s="6">
         <v>80</v>
       </c>
@@ -25327,7 +25331,7 @@
       </c>
       <c r="H974" s="6"/>
     </row>
-    <row r="975" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A975" s="6">
         <v>80</v>
       </c>
@@ -25349,7 +25353,7 @@
       </c>
       <c r="H975" s="6"/>
     </row>
-    <row r="976" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A976" s="6">
         <v>80</v>
       </c>
@@ -25371,7 +25375,7 @@
       </c>
       <c r="H976" s="6"/>
     </row>
-    <row r="977" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="977" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A977" s="6">
         <v>80</v>
       </c>
@@ -25393,7 +25397,7 @@
       </c>
       <c r="H977" s="6"/>
     </row>
-    <row r="978" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A978" s="6">
         <v>80</v>
       </c>
@@ -25415,7 +25419,7 @@
       </c>
       <c r="H978" s="6"/>
     </row>
-    <row r="979" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="979" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A979" s="6">
         <v>80</v>
       </c>
@@ -25437,7 +25441,7 @@
       </c>
       <c r="H979" s="6"/>
     </row>
-    <row r="980" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="980" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A980" s="6">
         <v>80</v>
       </c>
@@ -25459,7 +25463,7 @@
       </c>
       <c r="H980" s="6"/>
     </row>
-    <row r="981" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="981" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A981" s="6">
         <v>80</v>
       </c>
@@ -26077,7 +26081,7 @@
   <autoFilter ref="A1:H1007" xr:uid="{361EBCA0-C102-45D9-BE91-837AD7D26F73}">
     <filterColumn colId="2">
       <filters>
-        <filter val="talones_txt"/>
+        <filter val="update_BTM"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>